<commit_message>
updated - finished 6
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucy\Documents\DA15\Excel\lookups-exercise-cfazio93\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C3BDA9-6E44-44B3-AEBA-29B00FAF0B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15EC120-DF50-414F-97D9-989E1554151D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38640" yWindow="405" windowWidth="24480" windowHeight="20295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9180" yWindow="360" windowWidth="28380" windowHeight="20295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -1009,13 +1009,13 @@
                 <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>328800</c:v>
+                  <c:v>409300</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>334800</c:v>
+                  <c:v>428500</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>322700</c:v>
+                  <c:v>445200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1074,13 +1074,13 @@
                 <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>321214.59000000003</c:v>
+                  <c:v>385908.52</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>312433.70999999897</c:v>
+                  <c:v>427758.64</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>322263.03999999998</c:v>
+                  <c:v>445114.28999999899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2177,8 +2177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="K76" sqref="K76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2256,7 +2256,7 @@
         <v>341243679.13</v>
       </c>
       <c r="D2">
-        <f>C2 - B2</f>
+        <f t="shared" ref="D2:D33" si="0">C2 - B2</f>
         <v>-15396420.870000005</v>
       </c>
       <c r="E2" s="5">
@@ -2264,8 +2264,8 @@
         <v>-4.3170750765267295E-2</v>
       </c>
       <c r="F2" s="9">
-        <f>IFERROR(RANK(E2,E2:E52)," ")</f>
-        <v>35</v>
+        <f>IFERROR(RANK(E2,$E$2:$E$52, 1)," ")</f>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>382685200</v>
@@ -2274,7 +2274,7 @@
         <v>346340810.81999999</v>
       </c>
       <c r="I2">
-        <f>H2 - G2</f>
+        <f t="shared" ref="I2:I33" si="1">H2 - G2</f>
         <v>-36344389.180000007</v>
       </c>
       <c r="J2" s="5">
@@ -2282,7 +2282,7 @@
         <v>-9.4972027086493035E-2</v>
       </c>
       <c r="K2">
-        <f>IFERROR(RANK(J2, J2:J52), " ")</f>
+        <f>IFERROR(RANK(J2, $J$2:$J$52), " ")</f>
         <v>39</v>
       </c>
       <c r="L2">
@@ -2292,7 +2292,7 @@
         <v>355279492.22999901</v>
       </c>
       <c r="N2">
-        <f>M2 - L2</f>
+        <f t="shared" ref="N2:N33" si="2">M2 - L2</f>
         <v>-21269107.770000994</v>
       </c>
       <c r="O2" s="5">
@@ -2300,7 +2300,7 @@
         <v>-5.6484362894991494E-2</v>
       </c>
       <c r="P2">
-        <f>IFERROR(RANK(O2, O2:O52), " ")</f>
+        <f>IFERROR(RANK(O2, $O$2:$O$52), " ")</f>
         <v>35</v>
       </c>
     </row>
@@ -2315,16 +2315,16 @@
         <v>321214.59000000003</v>
       </c>
       <c r="D3">
-        <f>C3 - B3</f>
+        <f t="shared" si="0"/>
         <v>-7585.4099999999744</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E3:E52" si="0">IFERROR((D3 / B3), " ")</f>
+        <f t="shared" ref="E3:E52" si="3">IFERROR((D3 / B3), " ")</f>
         <v>-2.3069981751824741E-2</v>
       </c>
       <c r="F3" s="9">
-        <f t="shared" ref="F3:F52" si="1">IFERROR(RANK(E3,E3:E53)," ")</f>
-        <v>27</v>
+        <f t="shared" ref="F3:F52" si="4">IFERROR(RANK(E3,$E$2:$E$52, 1)," ")</f>
+        <v>22</v>
       </c>
       <c r="G3">
         <v>334800</v>
@@ -2333,15 +2333,15 @@
         <v>312433.70999999897</v>
       </c>
       <c r="I3">
-        <f>H3 - G3</f>
+        <f t="shared" si="1"/>
         <v>-22366.290000001027</v>
       </c>
       <c r="J3" s="5">
-        <f t="shared" ref="J3:J52" si="2">IFERROR((I3 / G3), " ")</f>
+        <f t="shared" ref="J3:J52" si="5">IFERROR((I3 / G3), " ")</f>
         <v>-6.6804928315415249E-2</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K52" si="3">IFERROR(RANK(J3, J3:J53), " ")</f>
+        <f t="shared" ref="K3:K52" si="6">IFERROR(RANK(J3, $J$2:$J$52), " ")</f>
         <v>35</v>
       </c>
       <c r="L3">
@@ -2351,15 +2351,15 @@
         <v>322263.03999999998</v>
       </c>
       <c r="N3">
-        <f>M3 - L3</f>
+        <f t="shared" si="2"/>
         <v>-436.96000000002095</v>
       </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O52" si="4">IFERROR((N3/L3), " ")</f>
+        <f t="shared" ref="O3:O52" si="7">IFERROR((N3/L3), " ")</f>
         <v>-1.3540749922529313E-3</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P52" si="5">IFERROR(RANK(O3, O3:O53), " ")</f>
+        <f t="shared" ref="P3:P52" si="8">IFERROR(RANK(O3, $O$2:$O$52), " ")</f>
         <v>12</v>
       </c>
     </row>
@@ -2374,16 +2374,16 @@
         <v>3115157.5599999898</v>
       </c>
       <c r="D4">
-        <f>C4 - B4</f>
+        <f t="shared" si="0"/>
         <v>-15442.440000010189</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4.9327413275443007E-3</v>
       </c>
       <c r="F4" s="9">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f t="shared" si="4"/>
+        <v>42</v>
       </c>
       <c r="G4">
         <v>3652300</v>
@@ -2392,15 +2392,15 @@
         <v>3589693.2099999902</v>
       </c>
       <c r="I4">
-        <f>H4 - G4</f>
+        <f t="shared" si="1"/>
         <v>-62606.790000009816</v>
       </c>
       <c r="J4" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1.7141743558856015E-2</v>
       </c>
       <c r="K4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="L4">
@@ -2410,16 +2410,16 @@
         <v>3564983.04999999</v>
       </c>
       <c r="N4">
-        <f>M4 - L4</f>
+        <f t="shared" si="2"/>
         <v>-97416.950000009965</v>
       </c>
       <c r="O4" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-2.6599210899959033E-2</v>
       </c>
       <c r="P4">
-        <f t="shared" si="5"/>
-        <v>23</v>
+        <f t="shared" si="8"/>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -2433,16 +2433,16 @@
         <v>6947552.6699999999</v>
       </c>
       <c r="D5">
-        <f>C5 - B5</f>
+        <f t="shared" si="0"/>
         <v>-723147.33000000007</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-9.4273968477453174E-2</v>
       </c>
       <c r="F5" s="9">
-        <f t="shared" si="1"/>
-        <v>42</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="G5">
         <v>7968300</v>
@@ -2451,16 +2451,16 @@
         <v>7020609.3200000003</v>
       </c>
       <c r="I5">
-        <f>H5 - G5</f>
+        <f t="shared" si="1"/>
         <v>-947690.6799999997</v>
       </c>
       <c r="J5" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-0.118932605449092</v>
       </c>
       <c r="K5">
-        <f t="shared" si="3"/>
-        <v>41</v>
+        <f t="shared" si="6"/>
+        <v>44</v>
       </c>
       <c r="L5">
         <v>7759600</v>
@@ -2469,16 +2469,16 @@
         <v>7497322.9100000001</v>
       </c>
       <c r="N5">
-        <f>M5 - L5</f>
+        <f t="shared" si="2"/>
         <v>-262277.08999999985</v>
       </c>
       <c r="O5" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-3.3800336357544182E-2</v>
       </c>
       <c r="P5">
-        <f t="shared" si="5"/>
-        <v>25</v>
+        <f t="shared" si="8"/>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -2492,16 +2492,16 @@
         <v>385908.52</v>
       </c>
       <c r="D6">
-        <f>C6 - B6</f>
+        <f t="shared" si="0"/>
         <v>-23391.479999999981</v>
       </c>
       <c r="E6" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-5.7149963352064452E-2</v>
       </c>
-      <c r="F6" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F6" s="9">
+        <f t="shared" si="4"/>
+        <v>11</v>
       </c>
       <c r="G6">
         <v>428500</v>
@@ -2510,15 +2510,15 @@
         <v>427758.64</v>
       </c>
       <c r="I6">
-        <f>H6 - G6</f>
+        <f t="shared" si="1"/>
         <v>-741.35999999998603</v>
       </c>
       <c r="J6" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1.7301283547257551E-3</v>
       </c>
       <c r="K6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="L6">
@@ -2528,15 +2528,15 @@
         <v>445114.28999999899</v>
       </c>
       <c r="N6">
-        <f>M6 - L6</f>
+        <f t="shared" si="2"/>
         <v>-85.710000001010485</v>
       </c>
       <c r="O6" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-1.925202156356929E-4</v>
       </c>
       <c r="P6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
     </row>
@@ -2551,16 +2551,16 @@
         <v>2946071.21</v>
       </c>
       <c r="D7">
-        <f>C7 - B7</f>
+        <f t="shared" si="0"/>
         <v>-382928.79000000004</v>
       </c>
       <c r="E7" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-0.11502817362571344</v>
       </c>
-      <c r="F7" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F7" s="9">
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>3390900</v>
@@ -2569,16 +2569,16 @@
         <v>3051483.41</v>
       </c>
       <c r="I7">
-        <f>H7 - G7</f>
+        <f t="shared" si="1"/>
         <v>-339416.58999999985</v>
       </c>
       <c r="J7" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-0.10009631366303927</v>
       </c>
       <c r="K7">
-        <f t="shared" si="3"/>
-        <v>37</v>
+        <f t="shared" si="6"/>
+        <v>41</v>
       </c>
       <c r="L7">
         <v>3345200</v>
@@ -2587,16 +2587,16 @@
         <v>2946440.08</v>
       </c>
       <c r="N7">
-        <f>M7 - L7</f>
+        <f t="shared" si="2"/>
         <v>-398759.91999999993</v>
       </c>
       <c r="O7" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.11920361114432618</v>
       </c>
       <c r="P7">
-        <f t="shared" si="5"/>
-        <v>40</v>
+        <f t="shared" si="8"/>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -2610,16 +2610,16 @@
         <v>1315623.30999999</v>
       </c>
       <c r="D8">
-        <f>C8 - B8</f>
+        <f t="shared" si="0"/>
         <v>-236476.69000000996</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-0.15235918433091292</v>
       </c>
-      <c r="F8" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F8" s="9">
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>1590700</v>
@@ -2628,16 +2628,16 @@
         <v>1383905.98999999</v>
       </c>
       <c r="I8">
-        <f>H8 - G8</f>
+        <f t="shared" si="1"/>
         <v>-206794.01000001002</v>
       </c>
       <c r="J8" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-0.13000189224870184</v>
       </c>
       <c r="K8">
-        <f t="shared" si="3"/>
-        <v>39</v>
+        <f t="shared" si="6"/>
+        <v>45</v>
       </c>
       <c r="L8">
         <v>1579300</v>
@@ -2646,16 +2646,16 @@
         <v>1337735.3199999901</v>
       </c>
       <c r="N8">
-        <f>M8 - L8</f>
+        <f t="shared" si="2"/>
         <v>-241564.68000000995</v>
       </c>
       <c r="O8" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.15295680364719175</v>
       </c>
       <c r="P8">
-        <f t="shared" si="5"/>
-        <v>41</v>
+        <f t="shared" si="8"/>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -2669,16 +2669,16 @@
         <v>8952825.2799999993</v>
       </c>
       <c r="D9">
-        <f>C9 - B9</f>
+        <f t="shared" si="0"/>
         <v>-396574.72000000067</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4.2417130511048909E-2</v>
       </c>
-      <c r="F9" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F9" s="9">
+        <f t="shared" si="4"/>
+        <v>16</v>
       </c>
       <c r="G9">
         <v>11073700</v>
@@ -2687,16 +2687,16 @@
         <v>9929059.5199999996</v>
       </c>
       <c r="I9">
-        <f>H9 - G9</f>
+        <f t="shared" si="1"/>
         <v>-1144640.4800000004</v>
       </c>
       <c r="J9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-0.10336567542917005</v>
       </c>
       <c r="K9">
-        <f t="shared" si="3"/>
-        <v>37</v>
+        <f t="shared" si="6"/>
+        <v>42</v>
       </c>
       <c r="L9">
         <v>10790500</v>
@@ -2705,16 +2705,16 @@
         <v>9993599.52999999</v>
       </c>
       <c r="N9">
-        <f>M9 - L9</f>
+        <f t="shared" si="2"/>
         <v>-796900.47000000998</v>
       </c>
       <c r="O9" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-7.3852043000788653E-2</v>
       </c>
       <c r="P9">
-        <f t="shared" si="5"/>
-        <v>35</v>
+        <f t="shared" si="8"/>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -2728,16 +2728,16 @@
         <v>407090.37</v>
       </c>
       <c r="D10">
-        <f>C10 - B10</f>
+        <f t="shared" si="0"/>
         <v>-36209.630000000005</v>
       </c>
       <c r="E10" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-8.1681998646514792E-2</v>
       </c>
-      <c r="F10" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F10" s="9">
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
       <c r="G10">
         <v>495200</v>
@@ -2746,16 +2746,16 @@
         <v>467907.84000000003</v>
       </c>
       <c r="I10">
-        <f>H10 - G10</f>
+        <f t="shared" si="1"/>
         <v>-27292.159999999974</v>
       </c>
       <c r="J10" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-5.5113408723747932E-2</v>
       </c>
       <c r="K10">
-        <f t="shared" si="3"/>
-        <v>30</v>
+        <f t="shared" si="6"/>
+        <v>32</v>
       </c>
       <c r="L10">
         <v>487500</v>
@@ -2764,16 +2764,16 @@
         <v>478318.92</v>
       </c>
       <c r="N10">
-        <f>M10 - L10</f>
+        <f t="shared" si="2"/>
         <v>-9181.0800000000163</v>
       </c>
       <c r="O10" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-1.883298461538465E-2</v>
       </c>
       <c r="P10">
-        <f t="shared" si="5"/>
-        <v>18</v>
+        <f t="shared" si="8"/>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -2787,15 +2787,15 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <f>C11 - B11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F11" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G11">
@@ -2805,15 +2805,15 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <f>H11 - G11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J11" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L11">
@@ -2823,16 +2823,16 @@
         <v>63771.91</v>
       </c>
       <c r="N11">
-        <f>M11 - L11</f>
+        <f t="shared" si="2"/>
         <v>-311228.08999999997</v>
       </c>
       <c r="O11" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.82994157333333329</v>
       </c>
       <c r="P11">
-        <f t="shared" si="5"/>
-        <v>39</v>
+        <f t="shared" si="8"/>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2846,16 +2846,16 @@
         <v>4066595.33</v>
       </c>
       <c r="D12">
-        <f>C12 - B12</f>
+        <f t="shared" si="0"/>
         <v>-214304.66999999993</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-5.0060657805601608E-2</v>
       </c>
-      <c r="F12" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F12" s="9">
+        <f t="shared" si="4"/>
+        <v>13</v>
       </c>
       <c r="G12">
         <v>4700400</v>
@@ -2864,16 +2864,16 @@
         <v>4205555.5999999996</v>
       </c>
       <c r="I12">
-        <f>H12 - G12</f>
+        <f t="shared" si="1"/>
         <v>-494844.40000000037</v>
       </c>
       <c r="J12" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-0.10527708280146378</v>
       </c>
       <c r="K12">
-        <f t="shared" si="3"/>
-        <v>36</v>
+        <f t="shared" si="6"/>
+        <v>43</v>
       </c>
       <c r="L12">
         <v>4677800</v>
@@ -2882,16 +2882,16 @@
         <v>4371713.1399999997</v>
       </c>
       <c r="N12">
-        <f>M12 - L12</f>
+        <f t="shared" si="2"/>
         <v>-306086.86000000034</v>
       </c>
       <c r="O12" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-6.5433934755654441E-2</v>
       </c>
       <c r="P12">
-        <f t="shared" si="5"/>
-        <v>33</v>
+        <f t="shared" si="8"/>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -2905,16 +2905,16 @@
         <v>5772288.3300000001</v>
       </c>
       <c r="D13">
-        <f>C13 - B13</f>
+        <f t="shared" si="0"/>
         <v>-75511.669999999925</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.2912833886247806E-2</v>
       </c>
-      <c r="F13" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F13" s="9">
+        <f t="shared" si="4"/>
+        <v>33</v>
       </c>
       <c r="G13">
         <v>6223700</v>
@@ -2923,16 +2923,16 @@
         <v>5909077.9399999902</v>
       </c>
       <c r="I13">
-        <f>H13 - G13</f>
+        <f t="shared" si="1"/>
         <v>-314622.06000000983</v>
       </c>
       <c r="J13" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-5.0552253482656594E-2</v>
       </c>
       <c r="K13">
-        <f t="shared" si="3"/>
-        <v>29</v>
+        <f t="shared" si="6"/>
+        <v>31</v>
       </c>
       <c r="L13">
         <v>6207300</v>
@@ -2941,16 +2941,16 @@
         <v>6056976.6699999999</v>
       </c>
       <c r="N13">
-        <f>M13 - L13</f>
+        <f t="shared" si="2"/>
         <v>-150323.33000000007</v>
       </c>
       <c r="O13" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-2.4217184605222895E-2</v>
       </c>
       <c r="P13">
-        <f t="shared" si="5"/>
-        <v>19</v>
+        <f t="shared" si="8"/>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -2964,16 +2964,16 @@
         <v>505017.37</v>
       </c>
       <c r="D14">
-        <f>C14 - B14</f>
+        <f t="shared" si="0"/>
         <v>-6982.6300000000047</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.3637949218750009E-2</v>
       </c>
-      <c r="F14" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F14" s="9">
+        <f t="shared" si="4"/>
+        <v>30</v>
       </c>
       <c r="G14">
         <v>530500</v>
@@ -2982,16 +2982,16 @@
         <v>524402.98</v>
       </c>
       <c r="I14">
-        <f>H14 - G14</f>
+        <f t="shared" si="1"/>
         <v>-6097.0200000000186</v>
       </c>
       <c r="J14" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1.1492968897266765E-2</v>
       </c>
       <c r="K14">
-        <f t="shared" si="3"/>
-        <v>8</v>
+        <f t="shared" si="6"/>
+        <v>9</v>
       </c>
       <c r="L14">
         <v>526200</v>
@@ -3000,16 +3000,16 @@
         <v>504989.88</v>
       </c>
       <c r="N14">
-        <f>M14 - L14</f>
+        <f t="shared" si="2"/>
         <v>-21210.119999999995</v>
       </c>
       <c r="O14" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-4.0308095781071827E-2</v>
       </c>
       <c r="P14">
-        <f t="shared" si="5"/>
-        <v>24</v>
+        <f t="shared" si="8"/>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -3023,16 +3023,16 @@
         <v>156545919.90000001</v>
       </c>
       <c r="D15">
-        <f>C15 - B15</f>
+        <f t="shared" si="0"/>
         <v>496819.90000000596</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.1837408866824991E-3</v>
       </c>
-      <c r="F15" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F15" s="9">
+        <f t="shared" si="4"/>
+        <v>48</v>
       </c>
       <c r="G15">
         <v>184167800</v>
@@ -3041,16 +3041,16 @@
         <v>175966389.24999899</v>
       </c>
       <c r="I15">
-        <f>H15 - G15</f>
+        <f t="shared" si="1"/>
         <v>-8201410.7500010133</v>
       </c>
       <c r="J15" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-4.4532273014072019E-2</v>
       </c>
       <c r="K15">
-        <f t="shared" si="3"/>
-        <v>22</v>
+        <f t="shared" si="6"/>
+        <v>25</v>
       </c>
       <c r="L15">
         <v>188953500</v>
@@ -3059,16 +3059,16 @@
         <v>184450910.84999901</v>
       </c>
       <c r="N15">
-        <f>M15 - L15</f>
+        <f t="shared" si="2"/>
         <v>-4502589.1500009894</v>
       </c>
       <c r="O15" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-2.3829085727446114E-2</v>
       </c>
       <c r="P15">
-        <f t="shared" si="5"/>
-        <v>18</v>
+        <f t="shared" si="8"/>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -3082,16 +3082,16 @@
         <v>6522480.4599999897</v>
       </c>
       <c r="D16">
-        <f>C16 - B16</f>
+        <f t="shared" si="0"/>
         <v>-78219.540000010282</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.1850188616360429E-2</v>
       </c>
-      <c r="F16" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F16" s="9">
+        <f t="shared" si="4"/>
+        <v>37</v>
       </c>
       <c r="G16">
         <v>7352500</v>
@@ -3100,15 +3100,15 @@
         <v>7350464.0800000001</v>
       </c>
       <c r="I16">
-        <f>H16 - G16</f>
+        <f t="shared" si="1"/>
         <v>-2035.9199999999255</v>
       </c>
       <c r="J16" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-2.769017341040361E-4</v>
       </c>
       <c r="K16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="L16">
@@ -3118,15 +3118,15 @@
         <v>7397093</v>
       </c>
       <c r="N16">
-        <f>M16 - L16</f>
+        <f t="shared" si="2"/>
         <v>-107</v>
       </c>
       <c r="O16" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-1.4464932677229222E-5</v>
       </c>
       <c r="P16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
     </row>
@@ -3141,16 +3141,16 @@
         <v>14439480.050000001</v>
       </c>
       <c r="D17">
-        <f>C17 - B17</f>
+        <f t="shared" si="0"/>
         <v>-421319.94999999925</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-2.8351094826658003E-2</v>
       </c>
-      <c r="F17" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F17" s="9">
+        <f t="shared" si="4"/>
+        <v>21</v>
       </c>
       <c r="G17">
         <v>15309700</v>
@@ -3159,16 +3159,16 @@
         <v>14645233.51</v>
       </c>
       <c r="I17">
-        <f>H17 - G17</f>
+        <f t="shared" si="1"/>
         <v>-664466.49000000022</v>
       </c>
       <c r="J17" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-4.3401666263871937E-2</v>
       </c>
       <c r="K17">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f t="shared" si="6"/>
+        <v>24</v>
       </c>
       <c r="L17">
         <v>15311800</v>
@@ -3177,16 +3177,16 @@
         <v>14346057.039999999</v>
       </c>
       <c r="N17">
-        <f>M17 - L17</f>
+        <f t="shared" si="2"/>
         <v>-965742.96000000089</v>
       </c>
       <c r="O17" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-6.3071811282801551E-2</v>
       </c>
       <c r="P17">
-        <f t="shared" si="5"/>
-        <v>28</v>
+        <f t="shared" si="8"/>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -3200,16 +3200,16 @@
         <v>2615303.8999999901</v>
       </c>
       <c r="D18">
-        <f>C18 - B18</f>
+        <f t="shared" si="0"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-5.4037002206391245E-2</v>
       </c>
-      <c r="F18" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F18" s="9">
+        <f t="shared" si="4"/>
+        <v>12</v>
       </c>
       <c r="G18">
         <v>2861000</v>
@@ -3218,16 +3218,16 @@
         <v>2671745.94</v>
       </c>
       <c r="I18">
-        <f>H18 - G18</f>
+        <f t="shared" si="1"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="J18" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-6.6149619014330668E-2</v>
       </c>
       <c r="K18">
-        <f t="shared" si="3"/>
-        <v>26</v>
+        <f t="shared" si="6"/>
+        <v>34</v>
       </c>
       <c r="L18">
         <v>2910600</v>
@@ -3236,16 +3236,16 @@
         <v>2535637.09</v>
       </c>
       <c r="N18">
-        <f>M18 - L18</f>
+        <f t="shared" si="2"/>
         <v>-374962.91000000015</v>
       </c>
       <c r="O18" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.12882667147667154</v>
       </c>
       <c r="P18">
-        <f t="shared" si="5"/>
-        <v>32</v>
+        <f t="shared" si="8"/>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -3259,16 +3259,16 @@
         <v>8460963.1999999899</v>
       </c>
       <c r="D19">
-        <f>C19 - B19</f>
+        <f t="shared" si="0"/>
         <v>-376336.80000001006</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4.258504294298146E-2</v>
       </c>
-      <c r="F19" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F19" s="9">
+        <f t="shared" si="4"/>
+        <v>15</v>
       </c>
       <c r="G19">
         <v>9713300</v>
@@ -3277,16 +3277,16 @@
         <v>8991707.2399999909</v>
       </c>
       <c r="I19">
-        <f>H19 - G19</f>
+        <f t="shared" si="1"/>
         <v>-721592.76000000909</v>
       </c>
       <c r="J19" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-7.4289145810384635E-2</v>
       </c>
       <c r="K19">
-        <f t="shared" si="3"/>
-        <v>27</v>
+        <f t="shared" si="6"/>
+        <v>37</v>
       </c>
       <c r="L19">
         <v>9343000</v>
@@ -3295,16 +3295,16 @@
         <v>8766655.9100000001</v>
       </c>
       <c r="N19">
-        <f>M19 - L19</f>
+        <f t="shared" si="2"/>
         <v>-576344.08999999985</v>
       </c>
       <c r="O19" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-6.1687262121374278E-2</v>
       </c>
       <c r="P19">
-        <f t="shared" si="5"/>
-        <v>27</v>
+        <f t="shared" si="8"/>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -3318,16 +3318,16 @@
         <v>124384360.159999</v>
       </c>
       <c r="D20">
-        <f>C20 - B20</f>
+        <f t="shared" si="0"/>
         <v>-1539.8400010019541</v>
       </c>
       <c r="E20" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.2379538203300809E-5</v>
       </c>
-      <c r="F20" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F20" s="9">
+        <f t="shared" si="4"/>
+        <v>46</v>
       </c>
       <c r="G20">
         <v>131849400</v>
@@ -3336,15 +3336,15 @@
         <v>131839624.37</v>
       </c>
       <c r="I20">
-        <f>H20 - G20</f>
+        <f t="shared" si="1"/>
         <v>-9775.6299999952316</v>
       </c>
       <c r="J20" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-7.4142392760188761E-5</v>
       </c>
       <c r="K20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="L20">
@@ -3354,15 +3354,15 @@
         <v>130621283.53999899</v>
       </c>
       <c r="N20">
-        <f>M20 - L20</f>
+        <f t="shared" si="2"/>
         <v>-116.46000100672245</v>
       </c>
       <c r="O20" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-8.9158438821450736E-7</v>
       </c>
       <c r="P20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
     </row>
@@ -3377,16 +3377,16 @@
         <v>22408587.5499999</v>
       </c>
       <c r="D21">
-        <f>C21 - B21</f>
+        <f t="shared" si="0"/>
         <v>-1923512.4500000998</v>
       </c>
       <c r="E21" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-7.9052463618023094E-2</v>
       </c>
-      <c r="F21" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F21" s="9">
+        <f t="shared" si="4"/>
+        <v>9</v>
       </c>
       <c r="G21">
         <v>24497400</v>
@@ -3395,16 +3395,16 @@
         <v>22655993.629999999</v>
       </c>
       <c r="I21">
-        <f>H21 - G21</f>
+        <f t="shared" si="1"/>
         <v>-1841406.370000001</v>
       </c>
       <c r="J21" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-7.5167420624229556E-2</v>
       </c>
       <c r="K21">
-        <f t="shared" si="3"/>
-        <v>26</v>
+        <f t="shared" si="6"/>
+        <v>38</v>
       </c>
       <c r="L21">
         <v>24323000</v>
@@ -3413,16 +3413,16 @@
         <v>23434073.089999899</v>
       </c>
       <c r="N21">
-        <f>M21 - L21</f>
+        <f t="shared" si="2"/>
         <v>-888926.91000010073</v>
       </c>
       <c r="O21" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-3.6546762734864152E-2</v>
       </c>
       <c r="P21">
-        <f t="shared" si="5"/>
-        <v>19</v>
+        <f t="shared" si="8"/>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -3436,16 +3436,16 @@
         <v>11412339.8799999</v>
       </c>
       <c r="D22">
-        <f>C22 - B22</f>
+        <f t="shared" si="0"/>
         <v>-153660.12000009976</v>
       </c>
       <c r="E22" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.3285502334437123E-2</v>
       </c>
-      <c r="F22" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F22" s="9">
+        <f t="shared" si="4"/>
+        <v>32</v>
       </c>
       <c r="G22">
         <v>11980700</v>
@@ -3454,16 +3454,16 @@
         <v>11791977.9699999</v>
       </c>
       <c r="I22">
-        <f>H22 - G22</f>
+        <f t="shared" si="1"/>
         <v>-188722.03000009991</v>
       </c>
       <c r="J22" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1.5752170574348738E-2</v>
       </c>
       <c r="K22">
-        <f t="shared" si="3"/>
-        <v>7</v>
+        <f t="shared" si="6"/>
+        <v>11</v>
       </c>
       <c r="L22">
         <v>11935200</v>
@@ -3472,16 +3472,16 @@
         <v>11934454.77</v>
       </c>
       <c r="N22">
-        <f>M22 - L22</f>
+        <f t="shared" si="2"/>
         <v>-745.23000000044703</v>
       </c>
       <c r="O22" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-6.2439674240938325E-5</v>
       </c>
       <c r="P22">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -3495,16 +3495,16 @@
         <v>20036743.4099999</v>
       </c>
       <c r="D23">
-        <f>C23 - B23</f>
+        <f t="shared" si="0"/>
         <v>-825956.59000010043</v>
       </c>
       <c r="E23" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-3.9590110100806722E-2</v>
       </c>
-      <c r="F23" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F23" s="9">
+        <f t="shared" si="4"/>
+        <v>18</v>
       </c>
       <c r="G23">
         <v>22683800</v>
@@ -3513,16 +3513,16 @@
         <v>21722126.219999898</v>
       </c>
       <c r="I23">
-        <f>H23 - G23</f>
+        <f t="shared" si="1"/>
         <v>-961673.78000010177</v>
       </c>
       <c r="J23" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-4.2394738976719144E-2</v>
       </c>
       <c r="K23">
-        <f t="shared" si="3"/>
-        <v>17</v>
+        <f t="shared" si="6"/>
+        <v>23</v>
       </c>
       <c r="L23">
         <v>23220300</v>
@@ -3531,16 +3531,16 @@
         <v>22619057.440000001</v>
       </c>
       <c r="N23">
-        <f>M23 - L23</f>
+        <f t="shared" si="2"/>
         <v>-601242.55999999866</v>
       </c>
       <c r="O23" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-2.5892971236375011E-2</v>
       </c>
       <c r="P23">
-        <f t="shared" si="5"/>
-        <v>15</v>
+        <f t="shared" si="8"/>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -3554,16 +3554,16 @@
         <v>904969.19</v>
       </c>
       <c r="D24">
-        <f>C24 - B24</f>
+        <f t="shared" si="0"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="E24" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.3334943305713101E-2</v>
       </c>
-      <c r="F24" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F24" s="9">
+        <f t="shared" si="4"/>
+        <v>31</v>
       </c>
       <c r="G24">
         <v>1112700</v>
@@ -3572,16 +3572,16 @@
         <v>1067214.42</v>
       </c>
       <c r="I24">
-        <f>H24 - G24</f>
+        <f t="shared" si="1"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="J24" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-4.087856565111897E-2</v>
       </c>
       <c r="K24">
-        <f t="shared" si="3"/>
-        <v>15</v>
+        <f t="shared" si="6"/>
+        <v>21</v>
       </c>
       <c r="L24">
         <v>1112600</v>
@@ -3590,16 +3590,16 @@
         <v>1112527.1200000001</v>
       </c>
       <c r="N24">
-        <f>M24 - L24</f>
+        <f t="shared" si="2"/>
         <v>-72.879999999888241</v>
       </c>
       <c r="O24" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-6.5504224339284781E-5</v>
       </c>
       <c r="P24">
-        <f t="shared" si="5"/>
-        <v>5</v>
+        <f t="shared" si="8"/>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -3613,16 +3613,16 @@
         <v>479149.53</v>
       </c>
       <c r="D25">
-        <f>C25 - B25</f>
+        <f t="shared" si="0"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="E25" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.0226130964676661E-2</v>
       </c>
-      <c r="F25" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F25" s="9">
+        <f t="shared" si="4"/>
+        <v>38</v>
       </c>
       <c r="G25">
         <v>505200</v>
@@ -3631,16 +3631,16 @@
         <v>497194.20999999897</v>
       </c>
       <c r="I25">
-        <f>H25 - G25</f>
+        <f t="shared" si="1"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="J25" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1.5846773555029746E-2</v>
       </c>
       <c r="K25">
-        <f t="shared" si="3"/>
-        <v>7</v>
+        <f t="shared" si="6"/>
+        <v>12</v>
       </c>
       <c r="L25">
         <v>496500</v>
@@ -3649,16 +3649,16 @@
         <v>494775.1</v>
       </c>
       <c r="N25">
-        <f>M25 - L25</f>
+        <f t="shared" si="2"/>
         <v>-1724.9000000000233</v>
       </c>
       <c r="O25" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-3.4741188318228064E-3</v>
       </c>
       <c r="P25">
-        <f t="shared" si="5"/>
-        <v>8</v>
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -3672,16 +3672,16 @@
         <v>4801960.08</v>
       </c>
       <c r="D26">
-        <f>C26 - B26</f>
+        <f t="shared" si="0"/>
         <v>-447839.91999999993</v>
       </c>
       <c r="E26" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-8.5306091660634673E-2</v>
       </c>
-      <c r="F26" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F26" s="9">
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
       <c r="G26">
         <v>5442200</v>
@@ -3690,16 +3690,16 @@
         <v>5122329.02999999</v>
       </c>
       <c r="I26">
-        <f>H26 - G26</f>
+        <f t="shared" si="1"/>
         <v>-319870.97000000998</v>
       </c>
       <c r="J26" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-5.8776040939327839E-2</v>
       </c>
       <c r="K26">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f t="shared" si="6"/>
+        <v>33</v>
       </c>
       <c r="L26">
         <v>5430700</v>
@@ -3708,16 +3708,16 @@
         <v>5117235.21</v>
       </c>
       <c r="N26">
-        <f>M26 - L26</f>
+        <f t="shared" si="2"/>
         <v>-313464.79000000004</v>
       </c>
       <c r="O26" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-5.7720881286022069E-2</v>
       </c>
       <c r="P26">
-        <f t="shared" si="5"/>
-        <v>20</v>
+        <f t="shared" si="8"/>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -3731,15 +3731,15 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <f>C27 - B27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E27" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F27" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G27">
@@ -3749,15 +3749,15 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <f>H27 - G27</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J27" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L27">
@@ -3767,15 +3767,15 @@
         <v>0</v>
       </c>
       <c r="N27">
-        <f>M27 - L27</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O27" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P27" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3790,16 +3790,16 @@
         <v>1250442.02</v>
       </c>
       <c r="D28">
-        <f>C28 - B28</f>
+        <f t="shared" si="0"/>
         <v>-132457.97999999998</v>
       </c>
       <c r="E28" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-9.5782760864849215E-2</v>
       </c>
-      <c r="F28" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F28" s="9">
+        <f t="shared" si="4"/>
+        <v>3</v>
       </c>
       <c r="G28">
         <v>1545700</v>
@@ -3808,16 +3808,16 @@
         <v>1281335.23</v>
       </c>
       <c r="I28">
-        <f>H28 - G28</f>
+        <f t="shared" si="1"/>
         <v>-264364.77</v>
       </c>
       <c r="J28" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-0.17103239309050916</v>
       </c>
       <c r="K28">
-        <f t="shared" si="3"/>
-        <v>23</v>
+        <f t="shared" si="6"/>
+        <v>47</v>
       </c>
       <c r="L28">
         <v>1525900</v>
@@ -3826,16 +3826,16 @@
         <v>1393285.06</v>
       </c>
       <c r="N28">
-        <f>M28 - L28</f>
+        <f t="shared" si="2"/>
         <v>-132614.93999999994</v>
       </c>
       <c r="O28" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-8.6909325643882263E-2</v>
       </c>
       <c r="P28">
-        <f t="shared" si="5"/>
-        <v>21</v>
+        <f t="shared" si="8"/>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -3849,16 +3849,16 @@
         <v>2523884.71</v>
       </c>
       <c r="D29">
-        <f>C29 - B29</f>
+        <f t="shared" si="0"/>
         <v>-37915.290000000037</v>
       </c>
       <c r="E29" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.4800253727847622E-2</v>
       </c>
-      <c r="F29" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F29" s="9">
+        <f t="shared" si="4"/>
+        <v>28</v>
       </c>
       <c r="G29">
         <v>2779500</v>
@@ -3867,16 +3867,16 @@
         <v>2665264.4399999902</v>
       </c>
       <c r="I29">
-        <f>H29 - G29</f>
+        <f t="shared" si="1"/>
         <v>-114235.56000000983</v>
       </c>
       <c r="J29" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-4.1099320021590155E-2</v>
       </c>
       <c r="K29">
-        <f t="shared" si="3"/>
-        <v>14</v>
+        <f t="shared" si="6"/>
+        <v>22</v>
       </c>
       <c r="L29">
         <v>2889900</v>
@@ -3885,16 +3885,16 @@
         <v>2889864.67</v>
       </c>
       <c r="N29">
-        <f>M29 - L29</f>
+        <f t="shared" si="2"/>
         <v>-35.330000000074506</v>
       </c>
       <c r="O29" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-1.2225336516860273E-5</v>
       </c>
       <c r="P29">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -3908,16 +3908,16 @@
         <v>12030494.1</v>
       </c>
       <c r="D30">
-        <f>C30 - B30</f>
+        <f t="shared" si="0"/>
         <v>-101705.90000000037</v>
       </c>
       <c r="E30" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-8.3831374359143746E-3</v>
       </c>
-      <c r="F30" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F30" s="9">
+        <f t="shared" si="4"/>
+        <v>40</v>
       </c>
       <c r="G30">
         <v>12735900</v>
@@ -3926,16 +3926,16 @@
         <v>12685514.279999901</v>
       </c>
       <c r="I30">
-        <f>H30 - G30</f>
+        <f t="shared" si="1"/>
         <v>-50385.720000099391</v>
       </c>
       <c r="J30" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-3.9561962641116366E-3</v>
       </c>
       <c r="K30">
-        <f t="shared" si="3"/>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>7</v>
       </c>
       <c r="L30">
         <v>12861300</v>
@@ -3944,16 +3944,16 @@
         <v>12826009.609999999</v>
       </c>
       <c r="N30">
-        <f>M30 - L30</f>
+        <f t="shared" si="2"/>
         <v>-35290.390000000596</v>
       </c>
       <c r="O30" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-2.7439209100169185E-3</v>
       </c>
       <c r="P30">
-        <f t="shared" si="5"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -3967,16 +3967,16 @@
         <v>1740827.69</v>
       </c>
       <c r="D31">
-        <f>C31 - B31</f>
+        <f t="shared" si="0"/>
         <v>-24772.310000000056</v>
       </c>
       <c r="E31" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.4030533529678329E-2</v>
       </c>
-      <c r="F31" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F31" s="9">
+        <f t="shared" si="4"/>
+        <v>29</v>
       </c>
       <c r="G31">
         <v>1823300</v>
@@ -3985,16 +3985,16 @@
         <v>1762676.85</v>
       </c>
       <c r="I31">
-        <f>H31 - G31</f>
+        <f t="shared" si="1"/>
         <v>-60623.149999999907</v>
       </c>
       <c r="J31" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-3.3249136181648611E-2</v>
       </c>
       <c r="K31">
-        <f t="shared" si="3"/>
-        <v>9</v>
+        <f t="shared" si="6"/>
+        <v>17</v>
       </c>
       <c r="L31">
         <v>1870700</v>
@@ -4003,16 +4003,16 @@
         <v>1801391.34</v>
       </c>
       <c r="N31">
-        <f>M31 - L31</f>
+        <f t="shared" si="2"/>
         <v>-69308.659999999916</v>
       </c>
       <c r="O31" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-3.7049585716576634E-2</v>
       </c>
       <c r="P31">
-        <f t="shared" si="5"/>
-        <v>13</v>
+        <f t="shared" si="8"/>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -4026,16 +4026,16 @@
         <v>5925637.7199999904</v>
       </c>
       <c r="D32">
-        <f>C32 - B32</f>
+        <f t="shared" si="0"/>
         <v>-73762.280000009574</v>
       </c>
       <c r="E32" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.2294942827617691E-2</v>
       </c>
-      <c r="F32" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F32" s="9">
+        <f t="shared" si="4"/>
+        <v>36</v>
       </c>
       <c r="G32">
         <v>6195500</v>
@@ -4044,16 +4044,16 @@
         <v>6084985.4699999997</v>
       </c>
       <c r="I32">
-        <f>H32 - G32</f>
+        <f t="shared" si="1"/>
         <v>-110514.53000000026</v>
       </c>
       <c r="J32" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1.7837871035428981E-2</v>
       </c>
       <c r="K32">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <f t="shared" si="6"/>
+        <v>14</v>
       </c>
       <c r="L32">
         <v>6157400</v>
@@ -4062,16 +4062,16 @@
         <v>5987572.0199999996</v>
       </c>
       <c r="N32">
-        <f>M32 - L32</f>
+        <f t="shared" si="2"/>
         <v>-169827.98000000045</v>
       </c>
       <c r="O32" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-2.7581118653977402E-2</v>
       </c>
       <c r="P32">
-        <f t="shared" si="5"/>
-        <v>12</v>
+        <f t="shared" si="8"/>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -4085,16 +4085,16 @@
         <v>920284264.73000002</v>
       </c>
       <c r="D33">
-        <f>C33 - B33</f>
+        <f t="shared" si="0"/>
         <v>-7418835.2699990273</v>
       </c>
       <c r="E33" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-7.9969930789269058E-3</v>
       </c>
-      <c r="F33" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F33" s="9">
+        <f t="shared" si="4"/>
+        <v>41</v>
       </c>
       <c r="G33">
         <v>979671000</v>
@@ -4103,16 +4103,16 @@
         <v>977068513.48000002</v>
       </c>
       <c r="I33">
-        <f>H33 - G33</f>
+        <f t="shared" si="1"/>
         <v>-2602486.5199999809</v>
       </c>
       <c r="J33" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-2.6564903115433454E-3</v>
       </c>
       <c r="K33">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="L33">
         <v>989572899.99999905</v>
@@ -4121,16 +4121,16 @@
         <v>984116289.40999901</v>
       </c>
       <c r="N33">
-        <f>M33 - L33</f>
+        <f t="shared" si="2"/>
         <v>-5456610.5900000334</v>
       </c>
       <c r="O33" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-5.5141067323084929E-3</v>
       </c>
       <c r="P33">
-        <f t="shared" si="5"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -4144,16 +4144,16 @@
         <v>4109958.22</v>
       </c>
       <c r="D34">
-        <f>C34 - B34</f>
+        <f t="shared" ref="D34:D52" si="9">C34 - B34</f>
         <v>-79341.779999999795</v>
       </c>
       <c r="E34" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.8939149738619768E-2</v>
       </c>
-      <c r="F34" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F34" s="9">
+        <f t="shared" si="4"/>
+        <v>26</v>
       </c>
       <c r="G34">
         <v>4350600</v>
@@ -4162,16 +4162,16 @@
         <v>4137588.7699999898</v>
       </c>
       <c r="I34">
-        <f>H34 - G34</f>
+        <f t="shared" ref="I34:I52" si="10">H34 - G34</f>
         <v>-213011.23000001023</v>
       </c>
       <c r="J34" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-4.8961345561534093E-2</v>
       </c>
       <c r="K34">
-        <f t="shared" si="3"/>
-        <v>12</v>
+        <f t="shared" si="6"/>
+        <v>28</v>
       </c>
       <c r="L34">
         <v>4345600</v>
@@ -4180,16 +4180,16 @@
         <v>4229801.51</v>
       </c>
       <c r="N34">
-        <f>M34 - L34</f>
+        <f t="shared" ref="N34:N52" si="11">M34 - L34</f>
         <v>-115798.49000000022</v>
       </c>
       <c r="O34" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-2.6647296115611244E-2</v>
       </c>
       <c r="P34">
-        <f t="shared" si="5"/>
-        <v>10</v>
+        <f t="shared" si="8"/>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -4203,15 +4203,15 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <f>C35 - B35</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E35" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F35" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G35">
@@ -4221,15 +4221,15 @@
         <v>0</v>
       </c>
       <c r="I35">
-        <f>H35 - G35</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J35" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="K35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L35">
@@ -4239,15 +4239,15 @@
         <v>0</v>
       </c>
       <c r="N35">
-        <f>M35 - L35</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="O35" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4262,16 +4262,16 @@
         <v>735423.27999999898</v>
       </c>
       <c r="D36">
-        <f>C36 - B36</f>
+        <f t="shared" si="9"/>
         <v>-62776.72000000102</v>
       </c>
       <c r="E36" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-7.8647857679780775E-2</v>
       </c>
-      <c r="F36" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F36" s="9">
+        <f t="shared" si="4"/>
+        <v>10</v>
       </c>
       <c r="G36">
         <v>898700</v>
@@ -4280,16 +4280,16 @@
         <v>740966.94999999902</v>
       </c>
       <c r="I36">
-        <f>H36 - G36</f>
+        <f t="shared" si="10"/>
         <v>-157733.05000000098</v>
       </c>
       <c r="J36" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-0.17551246244575608</v>
       </c>
       <c r="K36">
-        <f t="shared" si="3"/>
-        <v>17</v>
+        <f t="shared" si="6"/>
+        <v>48</v>
       </c>
       <c r="L36">
         <v>878300</v>
@@ -4298,16 +4298,16 @@
         <v>777215.28999999899</v>
       </c>
       <c r="N36">
-        <f>M36 - L36</f>
+        <f t="shared" si="11"/>
         <v>-101084.71000000101</v>
       </c>
       <c r="O36" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.11509132414892521</v>
       </c>
       <c r="P36">
-        <f t="shared" si="5"/>
-        <v>16</v>
+        <f t="shared" si="8"/>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -4321,16 +4321,16 @@
         <v>2005447.73999999</v>
       </c>
       <c r="D37">
-        <f>C37 - B37</f>
+        <f t="shared" si="9"/>
         <v>-82352.260000010021</v>
       </c>
       <c r="E37" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-3.9444515758219188E-2</v>
       </c>
-      <c r="F37" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F37" s="9">
+        <f t="shared" si="4"/>
+        <v>19</v>
       </c>
       <c r="G37">
         <v>2229200</v>
@@ -4339,16 +4339,16 @@
         <v>2118943.21</v>
       </c>
       <c r="I37">
-        <f>H37 - G37</f>
+        <f t="shared" si="10"/>
         <v>-110256.79000000004</v>
       </c>
       <c r="J37" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-4.9460250314014013E-2</v>
       </c>
       <c r="K37">
-        <f t="shared" si="3"/>
-        <v>12</v>
+        <f t="shared" si="6"/>
+        <v>29</v>
       </c>
       <c r="L37">
         <v>2296900</v>
@@ -4357,16 +4357,16 @@
         <v>2108718.34</v>
       </c>
       <c r="N37">
-        <f>M37 - L37</f>
+        <f t="shared" si="11"/>
         <v>-188181.66000000015</v>
       </c>
       <c r="O37" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-8.1928538464887526E-2</v>
       </c>
       <c r="P37">
-        <f t="shared" si="5"/>
-        <v>14</v>
+        <f t="shared" si="8"/>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -4380,16 +4380,16 @@
         <v>838669.82</v>
       </c>
       <c r="D38">
-        <f>C38 - B38</f>
+        <f t="shared" si="9"/>
         <v>-16630.180000000051</v>
       </c>
       <c r="E38" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.9443680579913542E-2</v>
       </c>
-      <c r="F38" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F38" s="9">
+        <f t="shared" si="4"/>
+        <v>25</v>
       </c>
       <c r="G38">
         <v>792800</v>
@@ -4398,16 +4398,16 @@
         <v>753451.96</v>
       </c>
       <c r="I38">
-        <f>H38 - G38</f>
+        <f t="shared" si="10"/>
         <v>-39348.040000000037</v>
       </c>
       <c r="J38" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-4.9631735620585316E-2</v>
       </c>
       <c r="K38">
-        <f t="shared" si="3"/>
-        <v>12</v>
+        <f t="shared" si="6"/>
+        <v>30</v>
       </c>
       <c r="L38">
         <v>777800</v>
@@ -4416,16 +4416,16 @@
         <v>777663.26</v>
       </c>
       <c r="N38">
-        <f>M38 - L38</f>
+        <f t="shared" si="11"/>
         <v>-136.73999999999069</v>
       </c>
       <c r="O38" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-1.7580354847003174E-4</v>
       </c>
       <c r="P38">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="8"/>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -4439,16 +4439,16 @@
         <v>813108.87</v>
       </c>
       <c r="D39">
-        <f>C39 - B39</f>
+        <f t="shared" si="9"/>
         <v>-70791.13</v>
       </c>
       <c r="E39" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-8.008952370177623E-2</v>
       </c>
-      <c r="F39" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F39" s="9">
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="G39">
         <v>1294400</v>
@@ -4457,16 +4457,16 @@
         <v>1114242.27999999</v>
       </c>
       <c r="I39">
-        <f>H39 - G39</f>
+        <f t="shared" si="10"/>
         <v>-180157.72000000998</v>
       </c>
       <c r="J39" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-0.13918241656366656</v>
       </c>
       <c r="K39">
-        <f t="shared" si="3"/>
-        <v>14</v>
+        <f t="shared" si="6"/>
+        <v>46</v>
       </c>
       <c r="L39">
         <v>1759500</v>
@@ -4475,16 +4475,16 @@
         <v>1680463.8699999901</v>
       </c>
       <c r="N39">
-        <f>M39 - L39</f>
+        <f t="shared" si="11"/>
         <v>-79036.1300000099</v>
       </c>
       <c r="O39" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-4.4919653310605226E-2</v>
       </c>
       <c r="P39">
-        <f t="shared" si="5"/>
-        <v>10</v>
+        <f t="shared" si="8"/>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -4498,16 +4498,16 @@
         <v>37565141.859999903</v>
       </c>
       <c r="D40">
-        <f>C40 - B40</f>
+        <f t="shared" si="9"/>
         <v>-816758.14000009745</v>
       </c>
       <c r="E40" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-2.1279773539092578E-2</v>
       </c>
-      <c r="F40" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F40" s="9">
+        <f t="shared" si="4"/>
+        <v>23</v>
       </c>
       <c r="G40">
         <v>39964900</v>
@@ -4516,16 +4516,16 @@
         <v>38095240.189999901</v>
       </c>
       <c r="I40">
-        <f>H40 - G40</f>
+        <f t="shared" si="10"/>
         <v>-1869659.8100000992</v>
       </c>
       <c r="J40" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-4.6782546934937892E-2</v>
       </c>
       <c r="K40">
-        <f t="shared" si="3"/>
-        <v>11</v>
+        <f t="shared" si="6"/>
+        <v>27</v>
       </c>
       <c r="L40">
         <v>40216700</v>
@@ -4534,16 +4534,16 @@
         <v>39606263.709999897</v>
       </c>
       <c r="N40">
-        <f>M40 - L40</f>
+        <f t="shared" si="11"/>
         <v>-610436.29000010341</v>
       </c>
       <c r="O40" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-1.5178676768608648E-2</v>
       </c>
       <c r="P40">
-        <f t="shared" si="5"/>
-        <v>7</v>
+        <f t="shared" si="8"/>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -4557,16 +4557,16 @@
         <v>4409060.2099999897</v>
       </c>
       <c r="D41">
-        <f>C41 - B41</f>
+        <f t="shared" si="9"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="E41" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-4.0110550149132493E-2</v>
       </c>
-      <c r="F41" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F41" s="9">
+        <f t="shared" si="4"/>
+        <v>17</v>
       </c>
       <c r="G41">
         <v>5089500</v>
@@ -4575,16 +4575,16 @@
         <v>4956043.6699999897</v>
       </c>
       <c r="I41">
-        <f>H41 - G41</f>
+        <f t="shared" si="10"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="J41" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-2.6221894095689226E-2</v>
       </c>
       <c r="K41">
-        <f t="shared" si="3"/>
-        <v>5</v>
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
       <c r="L41">
         <v>4799900</v>
@@ -4593,16 +4593,16 @@
         <v>4717822.6500000004</v>
       </c>
       <c r="N41">
-        <f>M41 - L41</f>
+        <f t="shared" si="11"/>
         <v>-82077.349999999627</v>
       </c>
       <c r="O41" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-1.7099804162586642E-2</v>
       </c>
       <c r="P41">
-        <f t="shared" si="5"/>
-        <v>7</v>
+        <f t="shared" si="8"/>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -4616,16 +4616,16 @@
         <v>188551675.67999899</v>
       </c>
       <c r="D42">
-        <f>C42 - B42</f>
+        <f t="shared" si="9"/>
         <v>-41624.320001006126</v>
       </c>
       <c r="E42" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-2.2070943135841053E-4</v>
       </c>
-      <c r="F42" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F42" s="9">
+        <f t="shared" si="4"/>
+        <v>44</v>
       </c>
       <c r="G42">
         <v>199130300</v>
@@ -4634,16 +4634,16 @@
         <v>196755033.31</v>
       </c>
       <c r="I42">
-        <f>H42 - G42</f>
+        <f t="shared" si="10"/>
         <v>-2375266.6899999976</v>
       </c>
       <c r="J42" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-1.1928203241796942E-2</v>
       </c>
       <c r="K42">
-        <f t="shared" si="3"/>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>10</v>
       </c>
       <c r="L42">
         <v>199954600</v>
@@ -4652,15 +4652,15 @@
         <v>199954563.74999899</v>
       </c>
       <c r="N42">
-        <f>M42 - L42</f>
+        <f t="shared" si="11"/>
         <v>-36.250001013278961</v>
       </c>
       <c r="O42" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-1.8129115815929696E-7</v>
       </c>
       <c r="P42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -4675,16 +4675,16 @@
         <v>7968645.8300000001</v>
       </c>
       <c r="D43">
-        <f>C43 - B43</f>
+        <f t="shared" si="9"/>
         <v>-166754.16999999993</v>
       </c>
       <c r="E43" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-2.0497353541313264E-2</v>
       </c>
-      <c r="F43" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F43" s="9">
+        <f t="shared" si="4"/>
+        <v>24</v>
       </c>
       <c r="G43">
         <v>8560800</v>
@@ -4693,16 +4693,16 @@
         <v>8171472.0199999996</v>
       </c>
       <c r="I43">
-        <f>H43 - G43</f>
+        <f t="shared" si="10"/>
         <v>-389327.98000000045</v>
       </c>
       <c r="J43" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-4.5477990374731388E-2</v>
       </c>
       <c r="K43">
-        <f t="shared" si="3"/>
-        <v>8</v>
+        <f t="shared" si="6"/>
+        <v>26</v>
       </c>
       <c r="L43">
         <v>8497500</v>
@@ -4711,16 +4711,16 @@
         <v>8150982.5699999901</v>
       </c>
       <c r="N43">
-        <f>M43 - L43</f>
+        <f t="shared" si="11"/>
         <v>-346517.43000000995</v>
       </c>
       <c r="O43" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-4.0778750220654303E-2</v>
       </c>
       <c r="P43">
-        <f t="shared" si="5"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -4734,16 +4734,16 @@
         <v>29789104.379999999</v>
       </c>
       <c r="D44">
-        <f>C44 - B44</f>
+        <f t="shared" si="9"/>
         <v>-294095.62000000104</v>
       </c>
       <c r="E44" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-9.7760750186150751E-3</v>
       </c>
-      <c r="F44" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F44" s="9">
+        <f t="shared" si="4"/>
+        <v>39</v>
       </c>
       <c r="G44">
         <v>31040700</v>
@@ -4752,16 +4752,16 @@
         <v>30793711.48</v>
       </c>
       <c r="I44">
-        <f>H44 - G44</f>
+        <f t="shared" si="10"/>
         <v>-246988.51999999955</v>
       </c>
       <c r="J44" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-7.9569249404813532E-3</v>
       </c>
       <c r="K44">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f t="shared" si="6"/>
+        <v>8</v>
       </c>
       <c r="L44">
         <v>31282200</v>
@@ -4770,16 +4770,16 @@
         <v>31282141.25</v>
       </c>
       <c r="N44">
-        <f>M44 - L44</f>
+        <f t="shared" si="11"/>
         <v>-58.75</v>
       </c>
       <c r="O44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-1.8780648419868168E-6</v>
       </c>
       <c r="P44">
-        <f t="shared" si="5"/>
-        <v>2</v>
+        <f t="shared" si="8"/>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -4793,16 +4793,16 @@
         <v>54589584.0499999</v>
       </c>
       <c r="D45">
-        <f>C45 - B45</f>
+        <f t="shared" si="9"/>
         <v>-712015.95000009984</v>
       </c>
       <c r="E45" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.287514194887851E-2</v>
       </c>
-      <c r="F45" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F45" s="9">
+        <f t="shared" si="4"/>
+        <v>34</v>
       </c>
       <c r="G45">
         <v>56792200</v>
@@ -4811,16 +4811,16 @@
         <v>54594953.959999897</v>
       </c>
       <c r="I45">
-        <f>H45 - G45</f>
+        <f t="shared" si="10"/>
         <v>-2197246.0400001034</v>
       </c>
       <c r="J45" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-3.8689222111488959E-2</v>
       </c>
       <c r="K45">
-        <f t="shared" si="3"/>
-        <v>5</v>
+        <f t="shared" si="6"/>
+        <v>19</v>
       </c>
       <c r="L45">
         <v>56027100</v>
@@ -4829,16 +4829,16 @@
         <v>55386549.6599999</v>
       </c>
       <c r="N45">
-        <f>M45 - L45</f>
+        <f t="shared" si="11"/>
         <v>-640550.34000010043</v>
       </c>
       <c r="O45" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-1.1432866237947358E-2</v>
       </c>
       <c r="P45">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="8"/>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -4852,16 +4852,16 @@
         <v>258322.43</v>
       </c>
       <c r="D46">
-        <f>C46 - B46</f>
+        <f t="shared" si="9"/>
         <v>-777.57000000000698</v>
       </c>
       <c r="E46" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-3.0010420686993711E-3</v>
       </c>
-      <c r="F46" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F46" s="9">
+        <f t="shared" si="4"/>
+        <v>43</v>
       </c>
       <c r="G46">
         <v>266000</v>
@@ -4870,16 +4870,16 @@
         <v>257402.90999999901</v>
       </c>
       <c r="I46">
-        <f>H46 - G46</f>
+        <f t="shared" si="10"/>
         <v>-8597.090000000986</v>
       </c>
       <c r="J46" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-3.2319887218048821E-2</v>
       </c>
       <c r="K46">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f t="shared" si="6"/>
+        <v>16</v>
       </c>
       <c r="L46">
         <v>267100</v>
@@ -4888,16 +4888,16 @@
         <v>254753.15999999901</v>
       </c>
       <c r="N46">
-        <f>M46 - L46</f>
+        <f t="shared" si="11"/>
         <v>-12346.840000000986</v>
       </c>
       <c r="O46" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-4.6225533508053113E-2</v>
       </c>
       <c r="P46">
-        <f t="shared" si="5"/>
-        <v>4</v>
+        <f t="shared" si="8"/>
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -4911,16 +4911,16 @@
         <v>70378426.719999999</v>
       </c>
       <c r="D47">
-        <f>C47 - B47</f>
+        <f t="shared" si="9"/>
         <v>-12273.280000001192</v>
       </c>
       <c r="E47" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.7435939690898361E-4</v>
       </c>
-      <c r="F47" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F47" s="9">
+        <f t="shared" si="4"/>
+        <v>45</v>
       </c>
       <c r="G47">
         <v>73467000</v>
@@ -4929,16 +4929,16 @@
         <v>73442541.659999996</v>
       </c>
       <c r="I47">
-        <f>H47 - G47</f>
+        <f t="shared" si="10"/>
         <v>-24458.340000003576</v>
       </c>
       <c r="J47" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-3.3291600310348285E-4</v>
       </c>
       <c r="K47">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f t="shared" si="6"/>
+        <v>4</v>
       </c>
       <c r="L47">
         <v>75072800</v>
@@ -4947,16 +4947,16 @@
         <v>75050829.179999903</v>
       </c>
       <c r="N47">
-        <f>M47 - L47</f>
+        <f t="shared" si="11"/>
         <v>-21970.820000097156</v>
       </c>
       <c r="O47" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-2.9266019117572752E-4</v>
       </c>
       <c r="P47">
-        <f t="shared" si="5"/>
-        <v>2</v>
+        <f t="shared" si="8"/>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -4970,16 +4970,16 @@
         <v>6527352.5699999901</v>
       </c>
       <c r="D48">
-        <f>C48 - B48</f>
+        <f t="shared" si="9"/>
         <v>-209747.43000000995</v>
       </c>
       <c r="E48" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-3.1133192323107857E-2</v>
       </c>
-      <c r="F48" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F48" s="9">
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
       <c r="G48">
         <v>7214700</v>
@@ -4988,16 +4988,16 @@
         <v>6922072.5599999996</v>
       </c>
       <c r="I48">
-        <f>H48 - G48</f>
+        <f t="shared" si="10"/>
         <v>-292627.44000000041</v>
       </c>
       <c r="J48" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-4.0559890224125802E-2</v>
       </c>
       <c r="K48">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f t="shared" si="6"/>
+        <v>20</v>
       </c>
       <c r="L48">
         <v>7289800</v>
@@ -5006,16 +5006,16 @@
         <v>6882350.23999999</v>
       </c>
       <c r="N48">
-        <f>M48 - L48</f>
+        <f t="shared" si="11"/>
         <v>-407449.76000001002</v>
       </c>
       <c r="O48" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-5.5893132870587676E-2</v>
       </c>
       <c r="P48">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f t="shared" si="8"/>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -5029,16 +5029,16 @@
         <v>90499.43</v>
       </c>
       <c r="D49">
-        <f>C49 - B49</f>
+        <f t="shared" si="9"/>
         <v>-1700.570000000007</v>
       </c>
       <c r="E49" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.8444360086767971E-2</v>
       </c>
-      <c r="F49" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F49" s="9">
+        <f t="shared" si="4"/>
+        <v>27</v>
       </c>
       <c r="G49">
         <v>102600</v>
@@ -5047,16 +5047,16 @@
         <v>95466.880000000005</v>
       </c>
       <c r="I49">
-        <f>H49 - G49</f>
+        <f t="shared" si="10"/>
         <v>-7133.1199999999953</v>
       </c>
       <c r="J49" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-6.9523586744639335E-2</v>
       </c>
       <c r="K49">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f t="shared" si="6"/>
+        <v>36</v>
       </c>
       <c r="L49">
         <v>0</v>
@@ -5065,15 +5065,15 @@
         <v>0</v>
       </c>
       <c r="N49">
-        <f>M49 - L49</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="O49" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="P49" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -5088,16 +5088,16 @@
         <v>832600</v>
       </c>
       <c r="D50">
-        <f>C50 - B50</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="E50" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F50" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F50" s="9">
+        <f t="shared" si="4"/>
+        <v>47</v>
       </c>
       <c r="G50">
         <v>859100</v>
@@ -5106,15 +5106,15 @@
         <v>859100</v>
       </c>
       <c r="I50">
-        <f>H50 - G50</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J50" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L50">
@@ -5124,15 +5124,15 @@
         <v>843200</v>
       </c>
       <c r="N50">
-        <f>M50 - L50</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="O50" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -5147,16 +5147,16 @@
         <v>8499425.3399999905</v>
       </c>
       <c r="D51">
-        <f>C51 - B51</f>
+        <f t="shared" si="9"/>
         <v>-110074.66000000946</v>
       </c>
       <c r="E51" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-1.2785255822058129E-2</v>
       </c>
-      <c r="F51" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F51" s="9">
+        <f t="shared" si="4"/>
+        <v>35</v>
       </c>
       <c r="G51">
         <v>8925500</v>
@@ -5165,16 +5165,16 @@
         <v>8599059.6199999992</v>
       </c>
       <c r="I51">
-        <f>H51 - G51</f>
+        <f t="shared" si="10"/>
         <v>-326440.38000000082</v>
       </c>
       <c r="J51" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-3.6573903982970231E-2</v>
       </c>
       <c r="K51">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>18</v>
       </c>
       <c r="L51">
         <v>8833900</v>
@@ -5183,16 +5183,16 @@
         <v>8735843.3100000005</v>
       </c>
       <c r="N51">
-        <f>M51 - L51</f>
+        <f t="shared" si="11"/>
         <v>-98056.689999999478</v>
       </c>
       <c r="O51" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-1.1100045280114048E-2</v>
       </c>
       <c r="P51">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" si="8"/>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -5206,16 +5206,16 @@
         <v>2254684.7999999998</v>
       </c>
       <c r="D52">
-        <f>C52 - B52</f>
+        <f t="shared" si="9"/>
         <v>-196315.20000000019</v>
       </c>
       <c r="E52" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-8.009596083231342E-2</v>
       </c>
-      <c r="F52" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+      <c r="F52" s="9">
+        <f t="shared" si="4"/>
+        <v>7</v>
       </c>
       <c r="G52">
         <v>2440700</v>
@@ -5224,16 +5224,16 @@
         <v>2204672.88</v>
       </c>
       <c r="I52">
-        <f>H52 - G52</f>
+        <f t="shared" si="10"/>
         <v>-236027.12000000011</v>
       </c>
       <c r="J52" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-9.6704683082722218E-2</v>
       </c>
       <c r="K52">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>40</v>
       </c>
       <c r="L52">
         <v>2321600</v>
@@ -5242,16 +5242,16 @@
         <v>2056835.26</v>
       </c>
       <c r="N52">
-        <f>M52 - L52</f>
+        <f t="shared" si="11"/>
         <v>-264764.74</v>
       </c>
       <c r="O52" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.11404408166781529</v>
       </c>
       <c r="P52">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" si="8"/>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -5283,75 +5283,94 @@
         <v>24</v>
       </c>
       <c r="B56">
-        <f>VLOOKUP($A56, A2:EP52, 4)</f>
+        <f>VLOOKUP($A56, $A$2:$P$52, 4, FALSE)</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C56">
-        <f>VLOOKUP($A56, A2:EP52, 9)</f>
+        <f>VLOOKUP($A56, $A$2:$P52, 9, FALSE)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D56">
-        <f>VLOOKUP($A56, A2:EP52, 14)</f>
+        <f>VLOOKUP($A56, $A$2:$P$52, 14, FALSE)</f>
         <v>-9181.0800000000163</v>
       </c>
-      <c r="E56" t="e">
-        <f>MATCH(A10, A2:D52, 0)</f>
+      <c r="E56" s="9">
+        <f>MATCH($A56, $A2:$A52, 0)</f>
+        <v>9</v>
+      </c>
+      <c r="F56" s="9">
+        <f>VLOOKUP($A56, A2:EP52, 4, 9)</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="G56" s="9" t="e">
+        <f t="shared" ref="G56:H56" si="12">VLOOKUP($A56, B2:EQ52, 4, 9)</f>
         <v>#N/A</v>
       </c>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
+      <c r="H56" s="9" t="e">
+        <f t="shared" si="12"/>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>25</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:B61" si="6">VLOOKUP($A57, A3:EP53, 4)</f>
+        <f t="shared" ref="B57:B61" si="13">VLOOKUP($A57, $A$2:$P$52, 4, FALSE)</f>
         <v>0</v>
       </c>
       <c r="C57">
-        <f t="shared" ref="C57:C61" si="7">VLOOKUP($A57, A3:EP53, 9)</f>
+        <f>VLOOKUP($A57, $A$2:$P53, 9, FALSE)</f>
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" ref="D57:D61" si="8">VLOOKUP($A57, A3:EP53, 14)</f>
+        <f t="shared" ref="D57:D61" si="14">VLOOKUP($A57, $A$2:$P$52, 14, FALSE)</f>
         <v>-311228.08999999997</v>
       </c>
-      <c r="F57" s="9"/>
+      <c r="F57" s="9">
+        <f t="shared" ref="F57:F58" si="15">VLOOKUP($A57, A3:EP53, 4, 9)</f>
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <f>VLOOKUP($A56, A2:EP52, 4)</f>
+        <v>-36209.630000000005</v>
+      </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>32</v>
       </c>
       <c r="B58">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C58">
-        <f t="shared" si="7"/>
+        <f>VLOOKUP($A58, $A$2:$P54, 9, FALSE)</f>
         <v>-189254.06000000006</v>
       </c>
       <c r="D58">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>-374962.91000000015</v>
       </c>
-      <c r="F58" s="9"/>
+      <c r="F58" s="9">
+        <f t="shared" si="15"/>
+        <v>-149396.10000000987</v>
+      </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>38</v>
       </c>
       <c r="B59">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C59">
-        <f t="shared" si="7"/>
+        <f>VLOOKUP($A59, $A$2:$P55, 9, FALSE)</f>
         <v>-45485.580000000075</v>
       </c>
       <c r="D59">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>-72.879999999888241</v>
       </c>
       <c r="F59" s="9"/>
@@ -5361,15 +5380,15 @@
         <v>39</v>
       </c>
       <c r="B60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C60">
-        <f t="shared" si="7"/>
+        <f>VLOOKUP($A60, $A$2:$P56, 9, FALSE)</f>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D60">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>-1724.9000000000233</v>
       </c>
       <c r="F60" s="9"/>
@@ -5379,15 +5398,15 @@
         <v>55</v>
       </c>
       <c r="B61">
-        <f t="shared" si="6"/>
+        <f t="shared" si="13"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C61">
-        <f t="shared" si="7"/>
+        <f>VLOOKUP($A61, $A$2:$P57, 9, FALSE)</f>
         <v>-133456.33000001032</v>
       </c>
       <c r="D61">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>-82077.349999999627</v>
       </c>
       <c r="F61" s="9"/>
@@ -5421,15 +5440,15 @@
         <v>24</v>
       </c>
       <c r="B65">
-        <f>_xlfn.XLOOKUP($A65,A2:A52, D2:D52)</f>
+        <f>_xlfn.XLOOKUP($A65,$A$2:$A$52, $D$2:$D$52)</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C65">
-        <f>_xlfn.XLOOKUP($A65,A2:A52, I2:I52)</f>
+        <f>_xlfn.XLOOKUP($A65,$A$2:$A$52, $I$2:$I$52)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D65">
-        <f>_xlfn.XLOOKUP($A65,A2:A52, N2:N52)</f>
+        <f>_xlfn.XLOOKUP($A65,$A$2:$A$52, $N$2:$N$52)</f>
         <v>-9181.0800000000163</v>
       </c>
       <c r="F65" s="9"/>
@@ -5439,15 +5458,15 @@
         <v>25</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B70" si="9">_xlfn.XLOOKUP($A66,A3:A53, D3:D53)</f>
+        <f t="shared" ref="B66:B70" si="16">_xlfn.XLOOKUP($A66,$A$2:$A$52, $D$2:$D$52)</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C70" si="10">_xlfn.XLOOKUP($A66,A3:A53, I3:I53)</f>
+        <f t="shared" ref="C66:C70" si="17">_xlfn.XLOOKUP($A66,$A$2:$A$52, $I$2:$I$52)</f>
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D70" si="11">_xlfn.XLOOKUP($A66,A3:A53, N3:N53)</f>
+        <f t="shared" ref="D66:D70" si="18">_xlfn.XLOOKUP($A66,$A$2:$A$52, $N$2:$N$52)</f>
         <v>-311228.08999999997</v>
       </c>
       <c r="F66" s="9"/>
@@ -5457,15 +5476,15 @@
         <v>32</v>
       </c>
       <c r="B67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D67">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>-374962.91000000015</v>
       </c>
       <c r="F67" s="9"/>
@@ -5475,15 +5494,15 @@
         <v>38</v>
       </c>
       <c r="B68">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C68">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D68">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>-72.879999999888241</v>
       </c>
       <c r="F68" s="9"/>
@@ -5493,15 +5512,15 @@
         <v>39</v>
       </c>
       <c r="B69">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C69">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>-1724.9000000000233</v>
       </c>
       <c r="F69" s="9"/>
@@ -5511,15 +5530,15 @@
         <v>55</v>
       </c>
       <c r="B70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C70">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D70">
-        <f t="shared" si="11"/>
+        <f t="shared" si="18"/>
         <v>-82077.349999999627</v>
       </c>
       <c r="F70" s="9"/>
@@ -5553,15 +5572,15 @@
         <v>24</v>
       </c>
       <c r="B74">
-        <f>INDEX(D2:D52,MATCH($A74,A2:A52,0))</f>
+        <f>INDEX($D$2:$D$52,MATCH($A74,$A$2:$A$52,0))</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C74">
-        <f>INDEX(I2:I52,MATCH($A74,A2:A52,0))</f>
+        <f>INDEX($I$2:$I$52,MATCH($A74,$A$2:$A$52,0))</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D74">
-        <f>INDEX(N2:N52,MATCH($A74,A2:A52,0))</f>
+        <f>INDEX($N$2:$N$52,MATCH($A74,$A$2:$A$52,0))</f>
         <v>-9181.0800000000163</v>
       </c>
       <c r="F74" s="9"/>
@@ -5571,15 +5590,15 @@
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="12">INDEX(D3:D53,MATCH($A75,A3:A53,0))</f>
+        <f t="shared" ref="B75:B79" si="19">INDEX($D$2:$D$52,MATCH($A75,$A$2:$A$52,0))</f>
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:C79" si="13">INDEX(I3:I53,MATCH($A75,A3:A53,0))</f>
+        <f t="shared" ref="C75:C79" si="20">INDEX($I$2:$I$52,MATCH($A75,$A$2:$A$52,0))</f>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:D79" si="14">INDEX(N3:N53,MATCH($A75,A3:A53,0))</f>
+        <f t="shared" ref="D75:D79" si="21">INDEX($N$2:$N$52,MATCH($A75,$A$2:$A$52,0))</f>
         <v>-311228.08999999997</v>
       </c>
       <c r="F75" s="9"/>
@@ -5589,15 +5608,15 @@
         <v>32</v>
       </c>
       <c r="B76">
-        <f t="shared" si="12"/>
+        <f t="shared" si="19"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C76">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D76">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>-374962.91000000015</v>
       </c>
       <c r="F76" s="9"/>
@@ -5607,15 +5626,15 @@
         <v>38</v>
       </c>
       <c r="B77">
-        <f t="shared" si="12"/>
+        <f t="shared" si="19"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C77">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D77">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>-72.879999999888241</v>
       </c>
       <c r="F77" s="9"/>
@@ -5625,15 +5644,15 @@
         <v>39</v>
       </c>
       <c r="B78">
-        <f t="shared" si="12"/>
+        <f t="shared" si="19"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D78">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>-1724.9000000000233</v>
       </c>
       <c r="F78" s="9"/>
@@ -5643,15 +5662,15 @@
         <v>55</v>
       </c>
       <c r="B79">
-        <f t="shared" si="12"/>
+        <f t="shared" si="19"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C79">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D79">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>-82077.349999999627</v>
       </c>
       <c r="F79" s="9"/>
@@ -5686,11 +5705,11 @@
       </c>
       <c r="B84" s="6">
         <f>INDEX(B2:B52,MATCH($B87,A2:A52,0))</f>
-        <v>328800</v>
+        <v>409300</v>
       </c>
       <c r="C84" s="6">
         <f>INDEX(C2:C52,MATCH($B87,A2:A52,0))</f>
-        <v>321214.59000000003</v>
+        <v>385908.52</v>
       </c>
       <c r="F84" s="9"/>
     </row>
@@ -5700,11 +5719,11 @@
       </c>
       <c r="B85" s="6">
         <f>INDEX(G2:G52,MATCH($B87,A2:A52,0))</f>
-        <v>334800</v>
+        <v>428500</v>
       </c>
       <c r="C85" s="6">
         <f>INDEX(H2:H52,MATCH($B87,A2:A52,0))</f>
-        <v>312433.70999999897</v>
+        <v>427758.64</v>
       </c>
       <c r="F85" s="9"/>
     </row>
@@ -5714,17 +5733,17 @@
       </c>
       <c r="B86" s="6">
         <f>INDEX(L2:L52,MATCH($B87,A2:A52,0))</f>
-        <v>322700</v>
+        <v>445200</v>
       </c>
       <c r="C86" s="6">
         <f>INDEX(M2:M52,MATCH($B87,A2:A52,0))</f>
-        <v>322263.03999999998</v>
+        <v>445114.28999999899</v>
       </c>
       <c r="F86" s="9"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F87" s="9"/>
     </row>
@@ -5863,7 +5882,7 @@
       <c r="I100" s="4"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>

</xml_diff>